<commit_message>
new data 29 04 2020
</commit_message>
<xml_diff>
--- a/data/CoronavirusUpdate_AllCountries_Public.xlsx
+++ b/data/CoronavirusUpdate_AllCountries_Public.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prognoz_Scheduled_Tasks\_MAINTENANCE\Covid19_Tracker\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="37010" windowHeight="18150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Country Updates" sheetId="2" r:id="rId1"/>
@@ -1999,7 +1999,7 @@
   <si>
     <t xml:space="preserve">The payment deadlines for local taxes (cars, building, and land) have been postponed to end of June with a 10% discount.
 Interest and penalties on due and outstanding fiscal obligations are suspended (until the end of the state of emergency + 30 days).
-New measures were announced on March 26, including tax deductions on the personal income tax and VAT exemptions on imports of medical and sanitary devices that can be used to prevent, limit and combat COVID-19.
+New measures were announced on March 26, including tax deductions on the corporate income tax and VAT exemptions on imports of medical and sanitary devices that can be used to prevent, limit and combat COVID-19.
 </t>
   </si>
   <si>
@@ -3351,28 +3351,28 @@
   </sheetPr>
   <dimension ref="A1:L160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" style="24" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="24" customWidth="1"/>
     <col min="2" max="2" width="15" style="24" customWidth="1"/>
-    <col min="3" max="3" width="36.1796875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="36.54296875" style="24" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="24" customWidth="1"/>
     <col min="6" max="6" width="28" style="24" customWidth="1"/>
-    <col min="7" max="7" width="59.81640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="67.54296875" style="24" customWidth="1"/>
-    <col min="9" max="9" width="53.54296875" style="24" customWidth="1"/>
-    <col min="10" max="10" width="66.54296875" style="24" customWidth="1"/>
-    <col min="11" max="11" width="45.54296875" style="24" customWidth="1"/>
-    <col min="12" max="12" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="24"/>
+    <col min="7" max="7" width="59.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="67.5703125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="53.5703125" style="24" customWidth="1"/>
+    <col min="10" max="10" width="66.5703125" style="24" customWidth="1"/>
+    <col min="11" max="11" width="45.5703125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3382,7 +3382,7 @@
       <c r="G1" s="4"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="G2" s="4"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="s">
@@ -3410,7 +3410,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" s="16" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="16" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="14" t="s">
         <v>4</v>
@@ -3444,12 +3444,12 @@
       </c>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" spans="1:12" s="17" customFormat="1" ht="187.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="17" customFormat="1" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>15</v>
@@ -3477,12 +3477,12 @@
       </c>
       <c r="L5" s="22"/>
     </row>
-    <row r="6" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>24</v>
@@ -3513,12 +3513,12 @@
       </c>
       <c r="L6" s="22"/>
     </row>
-    <row r="7" spans="1:12" s="17" customFormat="1" ht="300" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" s="17" customFormat="1" ht="318.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>34</v>
@@ -3549,12 +3549,12 @@
       </c>
       <c r="L7" s="22"/>
     </row>
-    <row r="8" spans="1:12" ht="350" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="369.75" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>44</v>
@@ -3585,12 +3585,12 @@
       </c>
       <c r="L8" s="22"/>
     </row>
-    <row r="9" spans="1:12" s="17" customFormat="1" ht="250" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" s="17" customFormat="1" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>54</v>
@@ -3621,12 +3621,12 @@
       </c>
       <c r="L9" s="22"/>
     </row>
-    <row r="10" spans="1:12" ht="187.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>64</v>
@@ -3657,12 +3657,12 @@
       </c>
       <c r="L10" s="22"/>
     </row>
-    <row r="11" spans="1:12" s="17" customFormat="1" ht="375" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" s="17" customFormat="1" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>73</v>
       </c>
       <c r="B11" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>74</v>
@@ -3693,12 +3693,12 @@
       </c>
       <c r="L11" s="22"/>
     </row>
-    <row r="12" spans="1:12" ht="350" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="382.5" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B12" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>84</v>
@@ -3729,12 +3729,12 @@
       </c>
       <c r="L12" s="22"/>
     </row>
-    <row r="13" spans="1:12" s="17" customFormat="1" ht="400" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>93</v>
       </c>
       <c r="B13" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>94</v>
@@ -3765,12 +3765,12 @@
       </c>
       <c r="L13" s="22"/>
     </row>
-    <row r="14" spans="1:12" ht="262.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="293.25" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>103</v>
       </c>
       <c r="B14" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>104</v>
@@ -3801,12 +3801,12 @@
       </c>
       <c r="L14" s="22"/>
     </row>
-    <row r="15" spans="1:12" s="17" customFormat="1" ht="162.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" s="17" customFormat="1" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B15" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>114</v>
@@ -3837,12 +3837,12 @@
       </c>
       <c r="L15" s="22"/>
     </row>
-    <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>123</v>
       </c>
       <c r="B16" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>124</v>
@@ -3873,12 +3873,12 @@
       </c>
       <c r="L16" s="22"/>
     </row>
-    <row r="17" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>133</v>
       </c>
       <c r="B17" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>134</v>
@@ -3909,12 +3909,12 @@
       </c>
       <c r="L17" s="22"/>
     </row>
-    <row r="18" spans="1:12" ht="312.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="344.25" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>143</v>
       </c>
       <c r="B18" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>144</v>
@@ -3945,12 +3945,12 @@
       </c>
       <c r="L18" s="22"/>
     </row>
-    <row r="19" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>153</v>
       </c>
       <c r="B19" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>154</v>
@@ -3981,12 +3981,12 @@
       </c>
       <c r="L19" s="22"/>
     </row>
-    <row r="20" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>163</v>
       </c>
       <c r="B20" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>164</v>
@@ -4017,12 +4017,12 @@
       </c>
       <c r="L20" s="22"/>
     </row>
-    <row r="21" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>173</v>
       </c>
       <c r="B21" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>174</v>
@@ -4053,12 +4053,12 @@
       </c>
       <c r="L21" s="22"/>
     </row>
-    <row r="22" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>183</v>
       </c>
       <c r="B22" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="23" t="s">
@@ -4081,12 +4081,12 @@
       </c>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" spans="1:12" s="17" customFormat="1" ht="125" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" s="17" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>189</v>
       </c>
       <c r="B23" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>190</v>
@@ -4114,12 +4114,12 @@
       </c>
       <c r="L23" s="22"/>
     </row>
-    <row r="24" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>198</v>
       </c>
       <c r="B24" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>199</v>
@@ -4150,12 +4150,12 @@
       </c>
       <c r="L24" s="22"/>
     </row>
-    <row r="25" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>208</v>
       </c>
       <c r="B25" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>209</v>
@@ -4186,12 +4186,12 @@
       </c>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" spans="1:12" ht="275" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
         <v>218</v>
       </c>
       <c r="B26" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>219</v>
@@ -4222,12 +4222,12 @@
       </c>
       <c r="L26" s="22"/>
     </row>
-    <row r="27" spans="1:12" s="17" customFormat="1" ht="150" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" s="17" customFormat="1" ht="153" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>228</v>
       </c>
       <c r="B27" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>229</v>
@@ -4253,12 +4253,12 @@
       </c>
       <c r="L27" s="22"/>
     </row>
-    <row r="28" spans="1:12" ht="237.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
         <v>236</v>
       </c>
       <c r="B28" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="23" t="s">
@@ -4287,12 +4287,12 @@
       </c>
       <c r="L28" s="22"/>
     </row>
-    <row r="29" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>245</v>
       </c>
       <c r="B29" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>246</v>
@@ -4323,12 +4323,12 @@
       </c>
       <c r="L29" s="22"/>
     </row>
-    <row r="30" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>255</v>
       </c>
       <c r="B30" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="23" t="s">
@@ -4355,12 +4355,12 @@
       </c>
       <c r="L30" s="22"/>
     </row>
-    <row r="31" spans="1:12" s="17" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" s="17" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>263</v>
       </c>
       <c r="B31" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>264</v>
@@ -4391,12 +4391,12 @@
       </c>
       <c r="L31" s="22"/>
     </row>
-    <row r="32" spans="1:12" ht="162.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>273</v>
       </c>
       <c r="B32" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>274</v>
@@ -4427,12 +4427,12 @@
       </c>
       <c r="L32" s="22"/>
     </row>
-    <row r="33" spans="1:12" s="17" customFormat="1" ht="387.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" s="17" customFormat="1" ht="395.25" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>283</v>
       </c>
       <c r="B33" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>284</v>
@@ -4463,12 +4463,12 @@
       </c>
       <c r="L33" s="22"/>
     </row>
-    <row r="34" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>293</v>
       </c>
       <c r="B34" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>294</v>
@@ -4499,12 +4499,12 @@
       </c>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:12" s="17" customFormat="1" ht="400" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" s="17" customFormat="1" ht="408" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>303</v>
       </c>
       <c r="B35" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>304</v>
@@ -4535,12 +4535,12 @@
       </c>
       <c r="L35" s="22"/>
     </row>
-    <row r="36" spans="1:12" ht="275" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
         <v>313</v>
       </c>
       <c r="B36" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>314</v>
@@ -4571,12 +4571,12 @@
       </c>
       <c r="L36" s="22"/>
     </row>
-    <row r="37" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>323</v>
       </c>
       <c r="B37" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>324</v>
@@ -4607,12 +4607,12 @@
       </c>
       <c r="L37" s="22"/>
     </row>
-    <row r="38" spans="1:12" ht="387.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="408" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
         <v>333</v>
       </c>
       <c r="B38" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="23" t="s">
@@ -4639,12 +4639,12 @@
       <c r="K38" s="23"/>
       <c r="L38" s="22"/>
     </row>
-    <row r="39" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>341</v>
       </c>
       <c r="B39" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C39" s="19" t="s">
         <v>342</v>
@@ -4675,12 +4675,12 @@
       </c>
       <c r="L39" s="22"/>
     </row>
-    <row r="40" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
         <v>351</v>
       </c>
       <c r="B40" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C40" s="22"/>
       <c r="D40" s="23" t="s">
@@ -4703,12 +4703,12 @@
       </c>
       <c r="L40" s="22"/>
     </row>
-    <row r="41" spans="1:12" s="17" customFormat="1" ht="400" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>357</v>
       </c>
       <c r="B41" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>358</v>
@@ -4739,12 +4739,12 @@
       </c>
       <c r="L41" s="22"/>
     </row>
-    <row r="42" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
         <v>367</v>
       </c>
       <c r="B42" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>368</v>
@@ -4775,12 +4775,12 @@
       </c>
       <c r="L42" s="22"/>
     </row>
-    <row r="43" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>377</v>
       </c>
       <c r="B43" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>378</v>
@@ -4811,12 +4811,12 @@
       </c>
       <c r="L43" s="22"/>
     </row>
-    <row r="44" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
         <v>387</v>
       </c>
       <c r="B44" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>388</v>
@@ -4847,12 +4847,12 @@
       </c>
       <c r="L44" s="22"/>
     </row>
-    <row r="45" spans="1:12" s="17" customFormat="1" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" s="17" customFormat="1" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>397</v>
       </c>
       <c r="B45" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>398</v>
@@ -4883,12 +4883,12 @@
       </c>
       <c r="L45" s="22"/>
     </row>
-    <row r="46" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="306" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
         <v>407</v>
       </c>
       <c r="B46" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>408</v>
@@ -4919,12 +4919,12 @@
       </c>
       <c r="L46" s="22"/>
     </row>
-    <row r="47" spans="1:12" s="17" customFormat="1" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" s="17" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>417</v>
       </c>
       <c r="B47" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>418</v>
@@ -4955,12 +4955,12 @@
       </c>
       <c r="L47" s="22"/>
     </row>
-    <row r="48" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
         <v>427</v>
       </c>
       <c r="B48" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>428</v>
@@ -4991,12 +4991,12 @@
       </c>
       <c r="L48" s="22"/>
     </row>
-    <row r="49" spans="1:12" s="17" customFormat="1" ht="300" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="17" customFormat="1" ht="306" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>437</v>
       </c>
       <c r="B49" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>438</v>
@@ -5021,12 +5021,12 @@
       </c>
       <c r="L49" s="22"/>
     </row>
-    <row r="50" spans="1:12" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
         <v>445</v>
       </c>
       <c r="B50" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C50" s="22"/>
       <c r="D50" s="23" t="s">
@@ -5051,12 +5051,12 @@
       <c r="K50" s="23"/>
       <c r="L50" s="22"/>
     </row>
-    <row r="51" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>452</v>
       </c>
       <c r="B51" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>453</v>
@@ -5087,12 +5087,12 @@
       </c>
       <c r="L51" s="22"/>
     </row>
-    <row r="52" spans="1:12" ht="212.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
         <v>462</v>
       </c>
       <c r="B52" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C52" s="22"/>
       <c r="D52" s="23" t="s">
@@ -5115,12 +5115,12 @@
       </c>
       <c r="L52" s="22"/>
     </row>
-    <row r="53" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>468</v>
       </c>
       <c r="B53" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>469</v>
@@ -5151,12 +5151,12 @@
       </c>
       <c r="L53" s="22"/>
     </row>
-    <row r="54" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
         <v>478</v>
       </c>
       <c r="B54" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>479</v>
@@ -5187,12 +5187,12 @@
       </c>
       <c r="L54" s="22"/>
     </row>
-    <row r="55" spans="1:12" s="17" customFormat="1" ht="250" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" s="17" customFormat="1" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>488</v>
       </c>
       <c r="B55" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="17" t="s">
@@ -5212,12 +5212,12 @@
       </c>
       <c r="L55" s="22"/>
     </row>
-    <row r="56" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>493</v>
       </c>
       <c r="B56" s="18">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>494</v>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="L56" s="22"/>
     </row>
-    <row r="57" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="18"/>
       <c r="C57" s="19"/>
       <c r="F57" s="20"/>
@@ -5257,7 +5257,7 @@
       <c r="J57" s="21"/>
       <c r="L57" s="22"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="23"/>
       <c r="B58" s="18"/>
       <c r="C58" s="22"/>
@@ -5271,7 +5271,7 @@
       <c r="K58" s="23"/>
       <c r="L58" s="22"/>
     </row>
-    <row r="59" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="18"/>
       <c r="C59" s="19"/>
       <c r="F59" s="20"/>
@@ -5280,7 +5280,7 @@
       <c r="J59" s="21"/>
       <c r="L59" s="22"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="23"/>
       <c r="B60" s="18"/>
       <c r="C60" s="22"/>
@@ -5294,7 +5294,7 @@
       <c r="K60" s="23"/>
       <c r="L60" s="22"/>
     </row>
-    <row r="61" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="18"/>
       <c r="C61" s="19"/>
       <c r="F61" s="20"/>
@@ -5303,7 +5303,7 @@
       <c r="J61" s="21"/>
       <c r="L61" s="22"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="23"/>
       <c r="B62" s="18"/>
       <c r="C62" s="22"/>
@@ -5317,7 +5317,7 @@
       <c r="K62" s="23"/>
       <c r="L62" s="22"/>
     </row>
-    <row r="63" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="18"/>
       <c r="C63" s="19"/>
       <c r="F63" s="20"/>
@@ -5326,7 +5326,7 @@
       <c r="J63" s="21"/>
       <c r="L63" s="22"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="23"/>
       <c r="B64" s="18"/>
       <c r="C64" s="22"/>
@@ -5340,7 +5340,7 @@
       <c r="K64" s="23"/>
       <c r="L64" s="22"/>
     </row>
-    <row r="65" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="18"/>
       <c r="C65" s="19"/>
       <c r="F65" s="20"/>
@@ -5349,7 +5349,7 @@
       <c r="J65" s="21"/>
       <c r="L65" s="22"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="23"/>
       <c r="B66" s="18"/>
       <c r="C66" s="22"/>
@@ -5363,7 +5363,7 @@
       <c r="K66" s="23"/>
       <c r="L66" s="22"/>
     </row>
-    <row r="67" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="18"/>
       <c r="C67" s="19"/>
       <c r="F67" s="20"/>
@@ -5372,7 +5372,7 @@
       <c r="J67" s="21"/>
       <c r="L67" s="22"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="23"/>
       <c r="B68" s="18"/>
       <c r="C68" s="22"/>
@@ -5386,7 +5386,7 @@
       <c r="K68" s="23"/>
       <c r="L68" s="22"/>
     </row>
-    <row r="69" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="18"/>
       <c r="C69" s="19"/>
       <c r="F69" s="20"/>
@@ -5395,7 +5395,7 @@
       <c r="J69" s="21"/>
       <c r="L69" s="22"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="23"/>
       <c r="B70" s="18"/>
       <c r="C70" s="22"/>
@@ -5409,7 +5409,7 @@
       <c r="K70" s="23"/>
       <c r="L70" s="22"/>
     </row>
-    <row r="71" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="18"/>
       <c r="C71" s="19"/>
       <c r="F71" s="20"/>
@@ -5418,7 +5418,7 @@
       <c r="J71" s="21"/>
       <c r="L71" s="22"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="23"/>
       <c r="B72" s="18"/>
       <c r="C72" s="22"/>
@@ -5432,7 +5432,7 @@
       <c r="K72" s="23"/>
       <c r="L72" s="22"/>
     </row>
-    <row r="73" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="18"/>
       <c r="C73" s="19"/>
       <c r="F73" s="20"/>
@@ -5441,7 +5441,7 @@
       <c r="J73" s="21"/>
       <c r="L73" s="22"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="23"/>
       <c r="B74" s="18"/>
       <c r="C74" s="22"/>
@@ -5455,7 +5455,7 @@
       <c r="K74" s="23"/>
       <c r="L74" s="22"/>
     </row>
-    <row r="75" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="18"/>
       <c r="C75" s="19"/>
       <c r="F75" s="20"/>
@@ -5464,7 +5464,7 @@
       <c r="J75" s="21"/>
       <c r="L75" s="22"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
       <c r="B76" s="18"/>
       <c r="C76" s="22"/>
@@ -5478,7 +5478,7 @@
       <c r="K76" s="23"/>
       <c r="L76" s="22"/>
     </row>
-    <row r="77" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="18"/>
       <c r="C77" s="19"/>
       <c r="F77" s="20"/>
@@ -5487,7 +5487,7 @@
       <c r="J77" s="21"/>
       <c r="L77" s="22"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="23"/>
       <c r="B78" s="18"/>
       <c r="C78" s="22"/>
@@ -5501,7 +5501,7 @@
       <c r="K78" s="23"/>
       <c r="L78" s="22"/>
     </row>
-    <row r="79" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="18"/>
       <c r="C79" s="19"/>
       <c r="F79" s="20"/>
@@ -5510,7 +5510,7 @@
       <c r="J79" s="21"/>
       <c r="L79" s="22"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="23"/>
       <c r="B80" s="18"/>
       <c r="C80" s="22"/>
@@ -5524,7 +5524,7 @@
       <c r="K80" s="23"/>
       <c r="L80" s="22"/>
     </row>
-    <row r="81" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="18"/>
       <c r="C81" s="19"/>
       <c r="F81" s="20"/>
@@ -5533,7 +5533,7 @@
       <c r="J81" s="21"/>
       <c r="L81" s="22"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="23"/>
       <c r="B82" s="18"/>
       <c r="C82" s="22"/>
@@ -5547,7 +5547,7 @@
       <c r="K82" s="23"/>
       <c r="L82" s="22"/>
     </row>
-    <row r="83" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="18"/>
       <c r="C83" s="19"/>
       <c r="F83" s="20"/>
@@ -5556,7 +5556,7 @@
       <c r="J83" s="21"/>
       <c r="L83" s="22"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="23"/>
       <c r="B84" s="18"/>
       <c r="C84" s="22"/>
@@ -5570,7 +5570,7 @@
       <c r="K84" s="23"/>
       <c r="L84" s="22"/>
     </row>
-    <row r="85" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="18"/>
       <c r="C85" s="19"/>
       <c r="F85" s="20"/>
@@ -5579,7 +5579,7 @@
       <c r="J85" s="21"/>
       <c r="L85" s="22"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="23"/>
       <c r="B86" s="18"/>
       <c r="C86" s="22"/>
@@ -5593,7 +5593,7 @@
       <c r="K86" s="23"/>
       <c r="L86" s="22"/>
     </row>
-    <row r="87" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="18"/>
       <c r="C87" s="19"/>
       <c r="F87" s="20"/>
@@ -5602,7 +5602,7 @@
       <c r="J87" s="21"/>
       <c r="L87" s="22"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="23"/>
       <c r="B88" s="18"/>
       <c r="C88" s="22"/>
@@ -5616,7 +5616,7 @@
       <c r="K88" s="23"/>
       <c r="L88" s="22"/>
     </row>
-    <row r="89" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="18"/>
       <c r="C89" s="19"/>
       <c r="F89" s="20"/>
@@ -5625,7 +5625,7 @@
       <c r="J89" s="21"/>
       <c r="L89" s="22"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="23"/>
       <c r="B90" s="18"/>
       <c r="C90" s="22"/>
@@ -5639,7 +5639,7 @@
       <c r="K90" s="23"/>
       <c r="L90" s="22"/>
     </row>
-    <row r="91" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="18"/>
       <c r="C91" s="19"/>
       <c r="F91" s="20"/>
@@ -5648,7 +5648,7 @@
       <c r="J91" s="21"/>
       <c r="L91" s="22"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="23"/>
       <c r="B92" s="18"/>
       <c r="C92" s="22"/>
@@ -5662,7 +5662,7 @@
       <c r="K92" s="23"/>
       <c r="L92" s="22"/>
     </row>
-    <row r="93" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="18"/>
       <c r="C93" s="19"/>
       <c r="F93" s="20"/>
@@ -5671,7 +5671,7 @@
       <c r="J93" s="21"/>
       <c r="L93" s="22"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="23"/>
       <c r="B94" s="18"/>
       <c r="C94" s="22"/>
@@ -5685,7 +5685,7 @@
       <c r="K94" s="23"/>
       <c r="L94" s="22"/>
     </row>
-    <row r="95" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="18"/>
       <c r="C95" s="19"/>
       <c r="F95" s="20"/>
@@ -5694,7 +5694,7 @@
       <c r="J95" s="21"/>
       <c r="L95" s="22"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="23"/>
       <c r="B96" s="18"/>
       <c r="C96" s="22"/>
@@ -5708,7 +5708,7 @@
       <c r="K96" s="23"/>
       <c r="L96" s="22"/>
     </row>
-    <row r="97" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="18"/>
       <c r="C97" s="19"/>
       <c r="F97" s="20"/>
@@ -5717,7 +5717,7 @@
       <c r="J97" s="21"/>
       <c r="L97" s="22"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="23"/>
       <c r="B98" s="18"/>
       <c r="C98" s="22"/>
@@ -5731,7 +5731,7 @@
       <c r="K98" s="23"/>
       <c r="L98" s="22"/>
     </row>
-    <row r="99" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="18"/>
       <c r="C99" s="19"/>
       <c r="F99" s="20"/>
@@ -5740,7 +5740,7 @@
       <c r="J99" s="21"/>
       <c r="L99" s="22"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="23"/>
       <c r="B100" s="18"/>
       <c r="C100" s="22"/>
@@ -5754,7 +5754,7 @@
       <c r="K100" s="23"/>
       <c r="L100" s="22"/>
     </row>
-    <row r="101" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="18"/>
       <c r="C101" s="19"/>
       <c r="F101" s="20"/>
@@ -5763,7 +5763,7 @@
       <c r="J101" s="21"/>
       <c r="L101" s="22"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="23"/>
       <c r="B102" s="18"/>
       <c r="C102" s="22"/>
@@ -5777,7 +5777,7 @@
       <c r="K102" s="23"/>
       <c r="L102" s="22"/>
     </row>
-    <row r="103" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="18"/>
       <c r="C103" s="19"/>
       <c r="F103" s="20"/>
@@ -5786,7 +5786,7 @@
       <c r="J103" s="21"/>
       <c r="L103" s="22"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="23"/>
       <c r="B104" s="18"/>
       <c r="C104" s="22"/>
@@ -5800,7 +5800,7 @@
       <c r="K104" s="23"/>
       <c r="L104" s="22"/>
     </row>
-    <row r="105" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="18"/>
       <c r="C105" s="19"/>
       <c r="F105" s="20"/>
@@ -5809,7 +5809,7 @@
       <c r="J105" s="21"/>
       <c r="L105" s="22"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="23"/>
       <c r="B106" s="18"/>
       <c r="C106" s="22"/>
@@ -5823,7 +5823,7 @@
       <c r="K106" s="23"/>
       <c r="L106" s="22"/>
     </row>
-    <row r="107" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="18"/>
       <c r="C107" s="19"/>
       <c r="F107" s="20"/>
@@ -5832,7 +5832,7 @@
       <c r="J107" s="21"/>
       <c r="L107" s="22"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="23"/>
       <c r="B108" s="18"/>
       <c r="C108" s="22"/>
@@ -5846,7 +5846,7 @@
       <c r="K108" s="23"/>
       <c r="L108" s="22"/>
     </row>
-    <row r="109" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="18"/>
       <c r="C109" s="19"/>
       <c r="F109" s="20"/>
@@ -5855,7 +5855,7 @@
       <c r="J109" s="21"/>
       <c r="L109" s="22"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="23"/>
       <c r="B110" s="18"/>
       <c r="C110" s="22"/>
@@ -5869,7 +5869,7 @@
       <c r="K110" s="23"/>
       <c r="L110" s="22"/>
     </row>
-    <row r="111" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="18"/>
       <c r="C111" s="19"/>
       <c r="F111" s="20"/>
@@ -5878,7 +5878,7 @@
       <c r="J111" s="21"/>
       <c r="L111" s="22"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="23"/>
       <c r="B112" s="18"/>
       <c r="C112" s="22"/>
@@ -5892,7 +5892,7 @@
       <c r="K112" s="23"/>
       <c r="L112" s="22"/>
     </row>
-    <row r="113" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="18"/>
       <c r="C113" s="19"/>
       <c r="F113" s="20"/>
@@ -5901,7 +5901,7 @@
       <c r="J113" s="21"/>
       <c r="L113" s="22"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="23"/>
       <c r="B114" s="18"/>
       <c r="C114" s="22"/>
@@ -5915,7 +5915,7 @@
       <c r="K114" s="23"/>
       <c r="L114" s="22"/>
     </row>
-    <row r="115" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="18"/>
       <c r="C115" s="19"/>
       <c r="F115" s="20"/>
@@ -5924,7 +5924,7 @@
       <c r="J115" s="21"/>
       <c r="L115" s="22"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="23"/>
       <c r="B116" s="18"/>
       <c r="C116" s="22"/>
@@ -5938,7 +5938,7 @@
       <c r="K116" s="23"/>
       <c r="L116" s="22"/>
     </row>
-    <row r="117" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="18"/>
       <c r="C117" s="19"/>
       <c r="F117" s="20"/>
@@ -5947,7 +5947,7 @@
       <c r="J117" s="21"/>
       <c r="L117" s="22"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="23"/>
       <c r="B118" s="18"/>
       <c r="C118" s="22"/>
@@ -5961,7 +5961,7 @@
       <c r="K118" s="23"/>
       <c r="L118" s="22"/>
     </row>
-    <row r="119" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="18"/>
       <c r="C119" s="19"/>
       <c r="F119" s="20"/>
@@ -5970,7 +5970,7 @@
       <c r="J119" s="21"/>
       <c r="L119" s="22"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="23"/>
       <c r="B120" s="18"/>
       <c r="C120" s="22"/>
@@ -5984,7 +5984,7 @@
       <c r="K120" s="23"/>
       <c r="L120" s="22"/>
     </row>
-    <row r="121" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="18"/>
       <c r="C121" s="19"/>
       <c r="F121" s="20"/>
@@ -5993,7 +5993,7 @@
       <c r="J121" s="21"/>
       <c r="L121" s="22"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
       <c r="B122" s="18"/>
       <c r="C122" s="22"/>
@@ -6007,7 +6007,7 @@
       <c r="K122" s="23"/>
       <c r="L122" s="22"/>
     </row>
-    <row r="123" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="18"/>
       <c r="C123" s="19"/>
       <c r="F123" s="20"/>
@@ -6016,7 +6016,7 @@
       <c r="J123" s="21"/>
       <c r="L123" s="22"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
       <c r="B124" s="18"/>
       <c r="C124" s="22"/>
@@ -6030,7 +6030,7 @@
       <c r="K124" s="23"/>
       <c r="L124" s="22"/>
     </row>
-    <row r="125" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="18"/>
       <c r="C125" s="19"/>
       <c r="F125" s="20"/>
@@ -6039,7 +6039,7 @@
       <c r="J125" s="21"/>
       <c r="L125" s="22"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="18"/>
       <c r="C126" s="22"/>
@@ -6053,7 +6053,7 @@
       <c r="K126" s="23"/>
       <c r="L126" s="22"/>
     </row>
-    <row r="127" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="18"/>
       <c r="C127" s="19"/>
       <c r="F127" s="20"/>
@@ -6062,7 +6062,7 @@
       <c r="J127" s="21"/>
       <c r="L127" s="22"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="23"/>
       <c r="B128" s="18"/>
       <c r="C128" s="22"/>
@@ -6076,7 +6076,7 @@
       <c r="K128" s="23"/>
       <c r="L128" s="22"/>
     </row>
-    <row r="129" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="18"/>
       <c r="C129" s="19"/>
       <c r="F129" s="20"/>
@@ -6085,7 +6085,7 @@
       <c r="J129" s="21"/>
       <c r="L129" s="22"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="23"/>
       <c r="B130" s="18"/>
       <c r="C130" s="22"/>
@@ -6099,7 +6099,7 @@
       <c r="K130" s="23"/>
       <c r="L130" s="22"/>
     </row>
-    <row r="131" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="18"/>
       <c r="C131" s="19"/>
       <c r="F131" s="20"/>
@@ -6108,7 +6108,7 @@
       <c r="J131" s="21"/>
       <c r="L131" s="22"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="23"/>
       <c r="B132" s="18"/>
       <c r="C132" s="22"/>
@@ -6122,7 +6122,7 @@
       <c r="K132" s="23"/>
       <c r="L132" s="22"/>
     </row>
-    <row r="133" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="18"/>
       <c r="C133" s="19"/>
       <c r="F133" s="20"/>
@@ -6131,85 +6131,85 @@
       <c r="J133" s="21"/>
       <c r="L133" s="22"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B134" s="18"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B135" s="18"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B136" s="18"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B137" s="18"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B138" s="18"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B139" s="18"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B140" s="18"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B141" s="18"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B142" s="18"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B143" s="18"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B144" s="18"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" s="18"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" s="18"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" s="18"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" s="18"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" s="18"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" s="18"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" s="18"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" s="18"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" s="18"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" s="18"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" s="18"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" s="18"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" s="18"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" s="18"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" s="18"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" s="18"/>
     </row>
   </sheetData>
@@ -6559,12 +6559,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new data + tacking GA codes
</commit_message>
<xml_diff>
--- a/data/CoronavirusUpdate_AllCountries_Public.xlsx
+++ b/data/CoronavirusUpdate_AllCountries_Public.xlsx
@@ -713,7 +713,8 @@
     <t>ESP</t>
   </si>
   <si>
-    <t xml:space="preserve">Mandated nation-wide quarantine for at least 15 days since March 15th, which has been further extended until April 11th. </t>
+    <t>• Mandated nation-wide quarantine for at least 15 days since March 15th, which has been further extended until April 11th. 
+• Ban on all non-essential work from March 30 to April 9, inclusive.</t>
   </si>
   <si>
     <t>• Land borders are closed except for Spanish citizens, residents and land transportation of goods (March 16). 
@@ -750,6 +751,7 @@
 • Supplemental credit of EUR 25 million to cover meal allowances to ensure the basic access to food for vulnerable children affected by the suspension of educational activity in schools.
 • Additional flexibility for local authorities to use their 2019 budgetary surplus to fund social services and primary assistance to dependent persons (EUR 300 million) 
 • The social benefit for energy provision (‘bono social’) will be automatically extended until September 15.
+• Dismissals for reasons realted to Covid19 will not be considered justified (from March 27 till the end of the health crisis)
 Other employment and social measures:
 • One-month credit postponement on mortgage payments for the most vulnerable.
 • Broadened scope for protected families in the supply of water and energy, which is ensured for vulnerable groups. Telecommunication services are also guaranteed.
@@ -1185,28 +1187,43 @@
     <t>The government has advised that indoor mass gatherings of 100 people or more and outdoor mass gatherings of more than 500 people should be cancelled. All State-run cultural institutions have closed, as have pubs. On 24 March, the government announced further containment measures, including i) all theatres, clubs, gyms/leisure centres, hairdressers, betting shops, marts, markets, casinos, bingo halls, libraries and other similar outlets to shut; ii) all hotels to limit occupancy to essential non-social and non-tourist reasons; iii) all non-essential retail outlets are to close to members of the public and all other retail outlets are to implement physical distancing
 all cafes and restaurants are to limit supply to take away food or delivery; iv) all sporting events are cancelled, including those behind closed doors
 all playgrounds and holiday/caravan parks will close; v) all places of worship are to restrict numbers entering at any one time to ensure adequate physical distancing
-all organised social indoor and outdoor events of any size are not to take place.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ireland has 2.8 intensive care unit beds per 1,000 inhabitants. This is low compared with many other European countries. For instance, Germany has six intensive care unit beds per 1,000 inhabitants (the highest across the European countries).   
-Critical pharmaceutical products and medicines are given a Customs 'green routing' to facilitate uninterrupted importation and supply.
-The government has allocated an extra EUR 435 million (around 0.2% of GNI*) to the Health Service Executive for improving capacity in the health service, increasing staffing and overtime, developing home testing and remote management solutions for mildly ill patients and pushing community awareness and preventive actions. The package will also be used to promote greater use of technology and telephone support. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A package of sick pay and illness/supplementary benefits to ensure that employees and the self-employed can abide by medical advice to self-isolate where appropriate, while having their income better protected than under current social welfare rules. This is estimated to cost up to €2.4 billion. Specific measures include:
-• Waiving the requirement for six waiting days for sick pay in respect of medically certified cases of self-isolation in accordance with public health guidelines. 
-• The removal of the means test requirement for Supplementary Welfare Allowance in respect of medically certified cases of self-isolation. 
-• The personal rate of Illness Benefit will be increased from €203 per week to €305 per week for a maximum period of two weeks of medically certified self-isolation, or for the duration of a person’s medically-certified absence from work due to Covid-19 diagnoses.
-• The self-employed will be entitled to receive either illness benefit or non-means tested supplementary welfare allowance. 
-• Delayed payment of local property tax if payed by annual debit instruction or single debit authority to 21 May 2020. 
-• Delay stamp duty on credit cards to 1 July 2020
-• Short-time work support payment for employees who have been temporarily placed on a shorter working week. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Financial supports have been announced, including a €200 million Strategic Banking Corporation of Ireland Working Capital scheme; a €200 million Rescue and Restructuring Scheme available through Enterprise Ireland for vulnerable but viable firms; the maximum loan available from Microfinance Ireland has been increased from €25,000 to €50,000 (these loans are now interest free with no repayments for 6 months); Local Enterprise Offices in every county will be providing vouchers from €2,500 up to €10,000; a Finance in Focus grant of €7,200 will be available to Enterprise Ireland and Údarás na Gaeltachta clients.
-The government has agreed with local authorities that they should defer business rates payments due from the most immediately affected businesses, primarily in the retail, hospitality, leisure and childcare sectors, until the end of May. 
-There have also been a variety of taxation measures to alleviate short-term difficulties. For example, i) interest on late payments is suspended for January/February VAT and both February and March PAYE (Employers) liabilities; ii) all debt enforcement activity is suspended until further notice; iii) current tax clearance status will remain in place for all businesses over the coming months; iv) the Relevant Contract Tax (RCT) rate review scheduled to take place this month (March) is suspended.
+all organised social indoor and outdoor events of any size are not to take place. On 27 March, the government advised that everybody should stay at home until 12 April 2020, except for the following situations:
+i) to travel to and from work, or for purposes of work, only where the work is an essential health, social care or other essential service and cannot be done from home
+to shop for essential food, beverage and household goods or collect a meal
+ii) to attend medical appointments and collect medicines and other health products
+for vital family reasons, such as providing care to children, elderly or vulnerable people
+iii) to take brief individual physical exercise within 2 kilometres of your home.
+iv) always observe 2 metres physical distancing
+v) you may take children from your own household outdoors for physical exercise
+vi) farming purposes, that is food production or care of animals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Irish health system was already experiencing significant challenges at the onset of the COVID-19 outbreak, but a number of measures are being put in place to support the delivery of health services at this critical time. These include agreement with GPs to ensure that cost is not a barrier to accessing services, the utilisation of private hospital capacity, and an expansion in both acute and community capacity. 
+The most recent data available at the onset of the crisis suggested Ireland had 2.8 acute care hospital beds per 1,000 inhabitants. This is low compared with many other European countries. For instance, Germany had six acute care beds per 1,000 inhabitants (the highest across the European countries).   
+The Government has allocated extra funding of the order of €1 billion (0.5% of GNI*) to the Health Service Executive for improving capacity in the health service, including using private hospital capacity, increasing staffing and overtime, developing home testing and remote management solutions for mildly ill patients and pushing community awareness and preventive actions. The package will also be used to promote greater use of technology and telephone support. Further health-related measures of a similar financial scale are under active consideration.
+To support public health policy, the Minister of Finance has increased the limit for contactless payments (to EUR 50 per transaction). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A package of sick pay and illness/supplementary benefits has been introduced to ensure that employees and the self-employed can abide by medical advice to self-isolate where appropriate, while having their income better protected than under current social welfare rules. For example, the government has waived the requirement for six waiting days for sick pay in respect of medically certified cases of self-isolation in accordance with public health guidelines and has removed the means test requirement for Supplementary Welfare Allowance in respect of medically certified cases of self-isolation. 
+There have also been measures announced to try and encourage businesses to keep workers in employment and to support those who have lost their jobs. On 24 March, the government announced: 
+i) a temporary wage subsidy of 70% of take home pay up to a maximum weekly tax free amount of EUR 410 per week to help affected companies keep paying their employees; 
+ii) workers who have lost their jobs due to the crisis will receive an enhanced emergency COVID-19 Pandemic Unemployment Payment of EUR 350 per week (an increase from EUR 203 per week); 
+iii) the COVID-19 Illness Payment will be increased to EUR 350 per week; 
+iv) the self-employed will be eligible for the COVID-19 Pandemic Unemployment Payment of EUR 350 directly from the Department of Employment Affairs and Social Protection.
+The government is also introducing legislation to prevent both the termination of residential tenancies and any rent increases for the duration of the COVID-19 crisis. Furthermore, the Commission for Regulation of Utilities has issued a moratorium on disconnections of domestic customers for non-payment to the gas and electricity suppliers.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The government has announced financial supports for businesses, including; 
+i) a €200 million Strategic Banking Corporation of Ireland Working Capital scheme; ii) a €200 million Rescue and Restructuring Scheme available through Enterprise Ireland for vulnerable but viable firms; iii) the Microfinance Ireland COVID-19 Loan includes an option for a moratorium on interest and repayments for the first six months; iv) Local Enterprise Offices in every county will be providing vouchers from €2,500 up to €10,000; v) a Finance in Focus grant of €7,200 will be available to Enterprise Ireland and Údarás na Gaeltachta clients.
+The government has also agreed with local authorities that they should defer business rates payments due from the most immediately affected businesses, primarily in the retail, hospitality, leisure and childcare sectors, until the end of May. 
+There have also been a variety of taxation measures to alleviate short-term difficulties. For example; i) interest on late payments has been suspended for January/February VAT and both February and March PAYE (Employers) liabilities; ii) all debt enforcement activity is suspended until further notice; iii) current tax clearance status will remain in place for all businesses over the coming months; iv) the Relevant Contract Tax rate review scheduled to take place this month (March) is suspended; v) critical pharmaceutical products and medicines will be given a Customs ‘green routing’ to facilitate uninterrupted importation and supply.
+Banking Initiatives 
+Following consultation with the Government and the Central Bank of Ireland, the Banking &amp; Payments Federation of Ireland (BPFI) members that includes the five retail Irish banks and main non-banks, have agreed a coordinated approach to assisting customers affected by COVID-19. These measures include:
+• a payment break for up to three months (to be followed by on-going reviews depending on the scale and extent of the situation) for all personal (including personal and buy-to-let mortgages), SME and corporate customers;   
+• seeking to ensure that such a payment break will not adversely impact the borrower’s credit record (the details of this to be discussed with the Central Bank of Ireland); and
+• banks and non-banks deferring court proceedings or any other enforcement action for three months.
 </t>
   </si>
   <si>
@@ -1248,8 +1265,8 @@
     <t>ISR</t>
   </si>
   <si>
-    <t>- As of 9 March all Israelis returning from abroad are ordered into a 14-day quarantine. This measure will be in effect for two weeks initially.
-'- partial lockdown (since 20 March): workplace restrictions with only around 30% of employees are allowed to go to work (since 20 March for 4 weeks). People are asked to stay home except for essential trips (e.g.work, food, medical appointments) (1 week initially). Enforcement has been strengthened recently</t>
+    <t xml:space="preserve">- As of 9 March all Israelis returning from abroad are ordered into a 14-day quarantine. This measure will be in effect for two weeks initially.
+'- partial lockdown (since 20 March, further tightened 25 March): People are ordered  to stay home except for essential trips (e.g.work, food, medical appointments) (to be reassessed every week). Workplace restrictions with only around 30% of employees being physically  allowed to go to work (since 20 March for 4 weeks). </t>
   </si>
   <si>
     <t xml:space="preserve">Since12 March all non-Israelis will be barred completely from entering Israel unless they can demonstrate that they have a place to self-isolate in Israel for 14 days. This extends previous measures that were confined to travellers from most affected countries in Asia and Europe. </t>
@@ -1265,36 +1282,40 @@
     <t>NIS 1 billion allocated to health system (11 March) to increase health sector capacity, including for the procurement of protective gear, medicine and respirators, to increase the number of hospital beds for corona virus patients and the number of tests for the virus.</t>
   </si>
   <si>
-    <t>A first emergency package of NIS 10 billion (0.7% of GDP) announced on 14 March, including NIS 1 billion for health sector, _x000D_NIS 1 billion for special needs (police, fire service, food security),_x000D_ fund for state guaranteed loans of NIS 8 billion to assist mainly SMEs with cash-flow problems (off balance sheet measure, increased from previously 4 billion announced on 10 March)_x000D_.
+    <t>A first emergency package of NIS 10 billion (0.7% of GDP) announced on 14 March, including NIS 1 billion for health sector, _x000D_NIS 1 billion for special needs (police, fire service, food security),_x000D_ fund for state guaranteed loans of NIS 8 billion for SMEs (off balance sheet measure)_x000D_.
 _x000D_
 Further measures announced on March 16 include broadened eligibility to unemployment benefits, tax deferals, grant for the self-employed._x000D_
 Overall support measures of around NIS 35 billion (2.5% of GDP).
 .</t>
   </si>
   <si>
-    <t xml:space="preserve">- All employees on involuntary unpaid leave for at least 30 days will be able to claim unemployment benefits after 1 day. Unemployment benefits can be claimed after employment for the least 6 months, from 12 months previously_x000D_. Unemployment benefits for tourist guides.
+    <t xml:space="preserve">- All employees on involuntary unpaid leave for at least 30 days will be able to claim unemployment benefits after 5 day. Unemployment benefits can be claimed after employment for the least 6 months, from 12 months previously_x000D_. Unemployment benefits for tourist guides.
+'- Grant of up to NIS 6000 for March and April for people over 67 years who quit a job (27 March)
 '- Ministry of Finance instructed banks to allow for a 4-months postponement of mortgage payments (15 March)
 </t>
   </si>
   <si>
-    <t>- Fund for state guaranteed loans of NIS 8 billion to assist mainly SMEs with cash-flow problems (increased from previously 4 billion announced on 10 March)_x000D_
+    <t>- Fund for state guaranteed loans of NIS 8 billion for SMEs (increased from previously NIS 4 billion announced on 10 March)_x000D_. Since 29 March, no interest payments for borrower in first year (state pays instead).  
 '- VAT, municipal taxes and social security contribution have been deferred for SMEs until the end April
-'-Grants of NIS 6,000 for all small businesses with annual turnover up to ILS 300,000 and self employed</t>
+'-Grants up to  NIS 6,000 for all small businesses and self employed. Criteria to be determined</t>
   </si>
   <si>
     <t>On 15 March BOI announced_x000D_
-'- start of purchasing government bonds of various types and maturities in the secondary market (later specified to totallying NIS 15 billion, 3.5% GDP)_x000D_
+'- start of purchasing government bonds of various types and maturities in the secondary market (on 23 March specified to totallying NIS 15 billion, 3.5% GDP)_x000D_
 - offering repo transactions to financial institutions with government bonds as collateral (undisclosed amount)_x000D_
 - a list of regulatory leniencies for banks (e.g. higher LTV for all purpose HH loans backed by real estats), aimed at preventing a tightening in credit conditions and to support the economy_x000D_
-18 March_x000D_ BOI announced
-- offering banks one-week US dollar swaps up to NIS 15 billion</t>
+-18 March_x000D_ BOI announced to offer banks one-week US dollar swaps up to NIS 15 billion. 
+-On 29 March the banking supervisor reduced the regulatory capital requirement for banks by 1 percentatge point</t>
   </si>
   <si>
     <t>ITA</t>
   </si>
   <si>
-    <t>- Nation-wide quarantine. “I stay at home decree”, aims at limiting the movement and contact of people. People are required to stay at home but can leave in case of necessity or justified motives. These movements were restricted on March 23 with fewer exceptions and a limited range of economic activities permitted to continue operating. 
-- Reconversion of facilities (e.g., army barracks) to host people in quarantine.</t>
+    <t xml:space="preserve">- 23 February: quarantine of municipalities with initial clusters of cases. 
+- 25 February: Restrictions introduced to several northern regions. 
+- 8 March: Quarantine extended across Lombardy and 14 other northern provinces. 
+- 9 March: Nation-wide quarantine. “I stay at home decree”, aims at limiting the movement and contact of people. People are required to stay at home but can leave in case of necessity or for prescribed motives. Reconversion of facilities (e.g., army barracks) to host people in quarantine.
+- 25 March: Movements restrictions reinforced, with fewer exceptions and a limited range of industrial and commercial activities permitted to continue operating, effective 29 March. </t>
   </si>
   <si>
     <t xml:space="preserve">Strict travel restrictions nation-wide, reinforced from March 23 to prohibit movements out of the municipality where individuals reside. </t>
@@ -1303,8 +1324,9 @@
     <t>Closure of schools and universities from March 4 until April 3</t>
   </si>
   <si>
-    <t>- Bars and restaurants along with many other retail trade activities (e.g. shopping centres; indoor and outdoor markets) closed from March 10 until 3 April, and all sporting competitions suspended over the same period along with other public gatherings.
-- All but prescribed essential production activities suspended from March 23, with the list of permitted activities further limited from March 26.</t>
+    <t xml:space="preserve">- Bars and restaurants along with many other retail trade activities (e.g. shopping centres; indoor and outdoor markets) closed from March 10 until 3 April, and all sporting competitions suspended over the same period along with other public gatherings.
+- All but prescribed essential production activities suspended from March 23, with the list of permitted activities further limited from March 26.
+- On March 30, closures extended from April 3 to 30 April for sports, bars and similar activities. </t>
   </si>
   <si>
     <t>EUR 3.2 billion for the national health service and to support civil protection. Within this package: 
@@ -3449,7 +3471,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>15</v>
@@ -3482,7 +3504,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>24</v>
@@ -3518,7 +3540,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>34</v>
@@ -3554,7 +3576,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>44</v>
@@ -3590,7 +3612,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>54</v>
@@ -3626,7 +3648,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>64</v>
@@ -3662,7 +3684,7 @@
         <v>73</v>
       </c>
       <c r="B11" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>74</v>
@@ -3698,7 +3720,7 @@
         <v>83</v>
       </c>
       <c r="B12" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>84</v>
@@ -3734,7 +3756,7 @@
         <v>93</v>
       </c>
       <c r="B13" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>94</v>
@@ -3770,7 +3792,7 @@
         <v>103</v>
       </c>
       <c r="B14" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>104</v>
@@ -3806,7 +3828,7 @@
         <v>113</v>
       </c>
       <c r="B15" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>114</v>
@@ -3842,7 +3864,7 @@
         <v>123</v>
       </c>
       <c r="B16" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>124</v>
@@ -3878,7 +3900,7 @@
         <v>133</v>
       </c>
       <c r="B17" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>134</v>
@@ -3914,7 +3936,7 @@
         <v>143</v>
       </c>
       <c r="B18" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>144</v>
@@ -3950,7 +3972,7 @@
         <v>153</v>
       </c>
       <c r="B19" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>154</v>
@@ -3986,7 +4008,7 @@
         <v>163</v>
       </c>
       <c r="B20" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>164</v>
@@ -4022,7 +4044,7 @@
         <v>173</v>
       </c>
       <c r="B21" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>174</v>
@@ -4058,7 +4080,7 @@
         <v>183</v>
       </c>
       <c r="B22" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="23" t="s">
@@ -4086,7 +4108,7 @@
         <v>189</v>
       </c>
       <c r="B23" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>190</v>
@@ -4119,7 +4141,7 @@
         <v>198</v>
       </c>
       <c r="B24" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>199</v>
@@ -4155,7 +4177,7 @@
         <v>208</v>
       </c>
       <c r="B25" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>209</v>
@@ -4191,7 +4213,7 @@
         <v>218</v>
       </c>
       <c r="B26" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>219</v>
@@ -4227,7 +4249,7 @@
         <v>228</v>
       </c>
       <c r="B27" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>229</v>
@@ -4258,7 +4280,7 @@
         <v>236</v>
       </c>
       <c r="B28" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="23" t="s">
@@ -4292,7 +4314,7 @@
         <v>245</v>
       </c>
       <c r="B29" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>246</v>
@@ -4328,7 +4350,7 @@
         <v>255</v>
       </c>
       <c r="B30" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="23" t="s">
@@ -4360,7 +4382,7 @@
         <v>263</v>
       </c>
       <c r="B31" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>264</v>
@@ -4391,12 +4413,12 @@
       </c>
       <c r="L31" s="22"/>
     </row>
-    <row r="32" spans="1:12" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>273</v>
       </c>
       <c r="B32" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>274</v>
@@ -4432,7 +4454,7 @@
         <v>283</v>
       </c>
       <c r="B33" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>284</v>
@@ -4468,7 +4490,7 @@
         <v>293</v>
       </c>
       <c r="B34" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>294</v>
@@ -4504,7 +4526,7 @@
         <v>303</v>
       </c>
       <c r="B35" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>304</v>
@@ -4540,7 +4562,7 @@
         <v>313</v>
       </c>
       <c r="B36" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>314</v>
@@ -4576,7 +4598,7 @@
         <v>323</v>
       </c>
       <c r="B37" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>324</v>
@@ -4612,7 +4634,7 @@
         <v>333</v>
       </c>
       <c r="B38" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="23" t="s">
@@ -4644,7 +4666,7 @@
         <v>341</v>
       </c>
       <c r="B39" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C39" s="19" t="s">
         <v>342</v>
@@ -4680,7 +4702,7 @@
         <v>351</v>
       </c>
       <c r="B40" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C40" s="22"/>
       <c r="D40" s="23" t="s">
@@ -4708,7 +4730,7 @@
         <v>357</v>
       </c>
       <c r="B41" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>358</v>
@@ -4744,7 +4766,7 @@
         <v>367</v>
       </c>
       <c r="B42" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>368</v>
@@ -4780,7 +4802,7 @@
         <v>377</v>
       </c>
       <c r="B43" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>378</v>
@@ -4816,7 +4838,7 @@
         <v>387</v>
       </c>
       <c r="B44" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>388</v>
@@ -4852,7 +4874,7 @@
         <v>397</v>
       </c>
       <c r="B45" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>398</v>
@@ -4888,7 +4910,7 @@
         <v>407</v>
       </c>
       <c r="B46" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>408</v>
@@ -4924,7 +4946,7 @@
         <v>417</v>
       </c>
       <c r="B47" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>418</v>
@@ -4960,7 +4982,7 @@
         <v>427</v>
       </c>
       <c r="B48" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>428</v>
@@ -4996,7 +5018,7 @@
         <v>437</v>
       </c>
       <c r="B49" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>438</v>
@@ -5026,7 +5048,7 @@
         <v>445</v>
       </c>
       <c r="B50" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C50" s="22"/>
       <c r="D50" s="23" t="s">
@@ -5056,7 +5078,7 @@
         <v>452</v>
       </c>
       <c r="B51" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>453</v>
@@ -5092,7 +5114,7 @@
         <v>462</v>
       </c>
       <c r="B52" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C52" s="22"/>
       <c r="D52" s="23" t="s">
@@ -5120,7 +5142,7 @@
         <v>468</v>
       </c>
       <c r="B53" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>469</v>
@@ -5156,7 +5178,7 @@
         <v>478</v>
       </c>
       <c r="B54" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>479</v>
@@ -5192,7 +5214,7 @@
         <v>488</v>
       </c>
       <c r="B55" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="17" t="s">
@@ -5217,7 +5239,7 @@
         <v>493</v>
       </c>
       <c r="B56" s="18">
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>494</v>

</xml_diff>

<commit_message>
data 30 03 18h
</commit_message>
<xml_diff>
--- a/data/CoronavirusUpdate_AllCountries_Public.xlsx
+++ b/data/CoronavirusUpdate_AllCountries_Public.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="504">
   <si>
     <t>Covid19 Update by Country</t>
   </si>
@@ -81,7 +81,7 @@
     <t>All schools and universities closed as of March 16</t>
   </si>
   <si>
-    <t>All shops and public spaces are closed from March 20 until 13 April, only supermarkets,small groceries shops, hardware stores and pharmacies as well as certain parts of public administration remain open.</t>
+    <t>All shops and public spaces are closed from March 20 until 13 April, only supermarkets, small groceries shops, hardware stores and pharmacies as well as certain parts of public administration remain open.</t>
   </si>
   <si>
     <t>The construction of 8 new emergency hospitals has been announced. The government is cooperating with domestic firms to increase the supply of respiratory equipment and has purchased 31,000 reagents to start decentralised testing throughout the country as of March 30. All workers in the health sector will receive a monthly bonus of 75 USD from April until July 2020. Prices for personal care, drugs and medical products have been fixed for 30 days. Exports of medical equipment necessary for the treatment of COVID infected patients require prior authorisation from the government.</t>
@@ -102,30 +102,28 @@
     <t xml:space="preserve">From 9pm AEDT 20 March 2020, only Australian citizens, residents and immediate family members can travel to Australia. All travellers to Australia are required to self-isolate for 14 days, either at home or in a hotel. Interstate travel is possible, but individual states have introduced a requirement to self isolate for 14 days after arrival. </t>
   </si>
   <si>
-    <t xml:space="preserve">Only Australian citizens, residents and immediate family members can travel to Australia. All Australians are not allowed to take a return trip overseas, unless in exceptional circumstances. Cruise ships from foreign ports are banned.  
+    <t xml:space="preserve">Only Australian citizens, residents and immediate family members can travel to Australia. However, from 28 March, all travellers arriving in Australia will be required to undertake their mandatory 14 day self-isolation at designated facilities. All Australians are not allowed to take a return trip overseas, unless in exceptional circumstances. Cruise ships from foreign ports are banned.  
 On 27 March 2020, the Western Australian government imposed restrictions on travel within the state. Western Australians will not be permitted to leave their regional boundary unless under exceptional circumstances (e.g. employment purposes, medical reasons, health and emergency services, people living in border communities, transport of essential goods, compassionate grounds). </t>
   </si>
   <si>
     <t>No national blanket closure of schools. Public schools in several sub-national jurisdictions have moved to online-only learning. Private and independent schools exercise discretion on closure and delivery methods.</t>
   </si>
   <si>
-    <t xml:space="preserve">The government has suspended non-essential gatherings. Essential gatherings are limited to 500 people for outdoor gatherings and 100 people for indoor gatherings. Where possible, people are advised to keep 1.5 metres between themself and others and there should be no more than one person per 4 square metres.
-On 25 March 2020, tighter restrictions were imposed on weddings, funerals, fitness classes, beauty salons, arcades, play centres. Pubs, licensed clubs and hotels (excluding accommodation), places of worship, gyms, indoor sporting venues, cinemas, casinos must close. Takeaway only at restaurants and cafes.
-</t>
-  </si>
-  <si>
-    <t>The Government has committed an additional $2.4 billion to support the health system to manage any further outbreak in Australia. The package provides support across primary care, aged care, hospitals, research and the National Medical Stockpile, along with a national communication campaign. The package also provides funding to ensure Australia has sufficient PPE and medicines in addition to infection control training and programs for health and aged care workers. On 15 March 2020, the Prime Minister announced that health services had moved into the ‘Targeted Action’ stage of the Australian Health Sector Emergency Response Plan for Novel Coronavirus (COVID-19). This included moving resources within hospitals to priority areas, establishing fever clinics which specialise in COVID-19, cancelling elective surgeries to free up capacity in public hospitals and adapting hospital resources (i.e. rooms and equipment) for use in priority areas, such as Intensive Care Units.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In addition to the Commonwealth Governments AUD$64bn package, state governments have also announced their own stimulus packages:
-• The Victorian government announced a AUD$1.7bn (0.1% of GDP) stimulus that included a fund to provide employment for some dismissed workers, payroll tax refunds for businesses and supports for firms in the worst-affected sectors. 
-• The New South Wales government announced a AUD$1.6bn (0.1% of GDP) package that included payroll tax relief for firms and new capital projects. 
-• The Queensland government have announced a AUD$3.2bn (0.2% of GDP) stimulus including the establishment of a loan facility for impacted businesses and payroll tax relief. 
-• The Western Australian government announced a AUD607mn package (0.03% of GDP) that included a freeze on household fees and charges and payroll tax relief for firms. 
-• The Tasmanian government announced a AUD$839mn (0.04% of GDP) package that included payments to households, interest free loans to small businesses and payroll tax waivers for businesses in sectors most heavily impacted and targeted industry assistance.
-• The South Australian government announced a $650 million jobs rescue package including a fund to provide employment opportunities, payroll tax relief, land tax relief, a once-off boost of $500 for households who are receiving the welfare support and a waiver of liquor licence fees for 2020-21 for those hotels, restaurants, cafes and clubs forced to close. 
-• The Australian Capital Territory announced a $137 million stimulus package targetting vulnerable households through cash payments and small business through the provision of credit and a fund for contractors to undertake simple works on government assets. 
-• The Northern Territory announced a $115 million stimulus package including payroll tax exemption, grants to businesses and not-for-profit and community organisations and a home improvement scheme. 
+    <t>The government (National Cabinet, made up of the Prime Minister, premiers and territory leaders) has now limited both indoor and outdoor gatherings to two persons only. Exceptions to this limit include: i) People of the same household going out together; ii) Funerals - a maximum of 10 people; iii) Wedding - a maximum of 5 people; iv) Family units. The government’s strong guidance to all Australians is to stay home unless for: i) shopping for what you need - food and necessary supplies; ii) medical or health care needs, including compassionate requirements; iii) exercise in compliance with the public gathering requirements; iv) work and study if you can’t work or learn remotely. The government has announced that playgrounds, skate parks and outside gyms in public places will be closed.</t>
+  </si>
+  <si>
+    <t>On 11 March, the Government committed an additional A$2.4 billion to support the health system to manage any further outbreak in Australia. The package provided support across primary care, aged care, hospitals, research and the National Medical Stockpile, along with a national communication campaign. The package also provided funding to ensure Australia had sufficient personal protective equipment and medicines in addition to infection control training and programs for health and aged care workers. On 15 March 2020, the Prime Minister announced that health services had moved into the ‘Targeted Action’ stage of the Australian Health Sector Emergency Response Plan for Novel Coronavirus (COVID-19). This included moving resources within hospitals to priority areas, establishing fever clinics which specialise in COVID-19, cancelling elective surgeries to free up capacity in public hospitals and adapting hospital resources (i.e. rooms and equipment) for use in priority areas, such as Intensive Care Units. On 29 March, the Prime Minister announced an additional A$1.1 billion in funding for mental health services, domestic violence support, Medicare assistance for people at home (including through telehealth services) and emergency food relief.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In addition to the Commonwealth Governments direct spending, state governments have announced their own stimulus packages:
+• The Victorian government announced a A$1.7bn (0.1% of GDP) stimulus that included a fund to provide employment for some dismissed workers, payroll tax refunds for businesses and supports for firms in the worst-affected sectors. 
+• The New South Wales government has announced two stimulus packages totalling around A$3bn (0.2% of GDP) package that included payroll tax relief for firms and new capital projects. 
+• The Queensland government have announced a A$4bn (0.2% of GDP) stimulus package including the establishment of a loan facility for impacted businesses, payroll tax relief and discount utility bills for households. 
+• The Western Australian government announced a A$607mn package (0.03% of GDP) that included a freeze on household fees and charges and payroll tax relief for firms. 
+• The Tasmanian government has announced approximately A$985mn (0.05% of GDP) in measures that includes payments to households, health spending, interest free loans to small businesses and payroll tax waivers for businesses in sectors most heavily impacted and targeted industry assistance.
+• The South Australian government has announced A$1bn (0.05% of GDP) in measures. These include a fund to provide employment opportunities, payroll tax relief, land tax relief, a one-off boost of A$500 for households who are receiving welfare support and a waiver of liquor licence fees for 2020-21 for those hotels, restaurants, cafes and clubs forced to close. 
+• The Australian Capital Territory announced a A$137 million stimulus package targeting vulnerable households through cash payments and small business through the provision of credit and a fund for contractors to undertake simple works on government assets. 
+• The Northern Territory announced a A$115 million stimulus package including payroll tax exemption, grants to businesses and not-for-profit and community organisations and a home improvement scheme.
 </t>
   </si>
   <si>
@@ -148,7 +146,7 @@
     <t>AUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Two popular ski regions (Paznauntal, St.Anton/Arlberg) in Tyrol have been under quarantine since March 13, the Gasteinertal, Grossarltal and Flachau (all in the Salzburg region), the rest of Tyrol, parts of Vorlarlberg (Lech, Warth, Schröcken, Klösterle, Nenzing-Dorf, Beschling) and Carinthia (Gemeinde Heiligenblut) since March 19.  </t>
+    <t>Two popular ski regions (Paznauntal, St.Anton/Arlberg) in Tyrol have been under quarantine since March 13, the Gasteinertal, Grossarltal and Flachau (all in the Salzburg region), the rest of Tyrol, parts of Vorlarlberg (Lech, Warth, Schröcken, Klösterle, Nenzing-Dorf, Beschling) and Carinthia (Gemeinde Heiligenblut) since March 19.  The quarantine in Heiligenblut (Carinthia) was lifted on Sunday March 29.</t>
   </si>
   <si>
     <t>The government has restricted access on Austria’s external borders for all neighbouring countries besides the Czech Republic and the Slovak Republic. However, both borders are closed from the respective other side, the Czech Republic restricts commuter traffic. Transit (and freight transport) is still possible. Official air traffic and external train traffic is suspended.</t>
@@ -160,7 +158,10 @@
     <t>Austrian authorities have enforced a country-wide curfew since 16 March. As of 10 March, big indoor and outdoor events have been cancelled and the government closed the external border with Italy. On 13 March, authorities announced the closure of schools from 16 March on and closed all shops besides supermarkets, pharmacies and a couple of other essential shops (a full list of businesses still allowed to open is found here). Museums, monuments, restaurants and bars are also closed. All events with more than five people are prohibited. In addition, municipal council elections in Styria and Vorarlberg (initially scheduled for 22/03) have been postponed until further notice.</t>
   </si>
   <si>
-    <t xml:space="preserve">Due to the closed borders especially with Hungary and Slovakia, maintaining 24h long-term care of the elderly is a major problem. Around 66,000 care-takers work in the labour-intensive 24h care. Austrians constitute only 1.6% of 24h care-takers. Around 50% of these care-takers come from Romania who currently cannot cross the Hungarian border and a further 30% from the Slovak Republic. Slovaks, the second largest group among care-takers, are only allowed to enter if their place of work is not more than 30km from the border. Though the Austrian government is in negotiations with its neighbours no solution has been reached so far. For the moment, the government has introduced two immediate measures for the 460.000 persons in need of care. Firstly, the government is seeking former Civilian Servants who completed their service within the last five years to step in. While this pool amounts to around 45,000 persons, the government estimates that about 14.600 additional Civilian Servants can be mobilized this way, who are also needed in other areas. Secondly, federal provinces are setting up additional capacities for mobile and stationary care, financed through a EUR 100 million fund from the federal government. Another 60 million are granted to the health system and EUR 130 million are given to hospitals for equipment and to finance over-time payments. A number of hotlines have been set up to provide Austrian with up-to-date and free info on the corona virus. The Ministry of Social Affairs, Health, Care and Consumer Protection set up a taskforce to provide scientific advice from a medial point of view. </t>
+    <t xml:space="preserve">Due to the closed borders especially with Hungary and Slovakia, maintaining 24h long-term care of the elderly is a major problem. Around 66,000 care-takers work in the labour-intensive 24h care. Austrians constitute only 1.6% of 24h care-takers. Around 50% of these care-takers come from Romania who currently cannot cross the Hungarian border and a further 30% from the Slovak Republic. Slovaks, the second largest group among care-takers, are only allowed to enter if their place of work is not more than 30km from the border. Though the Austrian government is in negotiations with its neighbours no solution has been reached so far. 
+For the moment, the government has introduced two immediate measures for the 460.000 persons in need of care. Firstly, the government is seeking former Civilian Servants who completed their service within the last five years to step in. While this pool amounts to around 45,000 persons, the government estimates that about 14.600 additional Civilian Servants can be mobilized this way, who are also needed in other areas. Secondly, federal provinces are setting up additional capacities for mobile and stationary care, financed through a EUR 100 million fund from the federal government. Another 60 million are granted to the health system and EUR 130 million are given to hospitals for equipment and to finance over-time payments. On Monday (March 30), Lower Austria announced that it will fly in 250 care-takes from Bulgaria and Romania. 
+From Wednesday April 1 on, the government has introduced further measures to contain the propagation of the virus. Wearing masks will be mandatory in open spaces, including supermarkets. Vulnerable people have to work from home. Hotels will be closed for tourists. Moreover, the government is currently undertaking testing of a representative sample of Austrians to get a more reliable estimate of the number of people infected with the virus.
+</t>
   </si>
   <si>
     <t>Chancellor Kurz has announced a comprehensive support package on 18 March amounting to up to EUR 38 Billion (around 10% of GDP but including tax deferals). The package encompasses credit guarantees of EUR 9 billion, a compartment for immediate help of EUR 4 billion, including EUR 400 million for short-time work via the Public Employment Service Austria (AMS), tax deferrals of up to EUR 10 billion and EUR 15 billion in form of credit guarantees and subsidies for hard-hit industries. Firms affected can claim a deferral of social contributions for the months February to April. Additional funds will be put aside to support the production of gloves, masks and several medicines in Austria. Further EUR 23 million are disbursed through an emergency-call for research by the Austrian Research Promotion Agency (FFG) to incentivize eligible research on Covid-19 by Austrian firms.</t>
@@ -226,19 +227,19 @@
     <t>Overseas arrivals from high-risk countries required to self-isolate for 14 days.</t>
   </si>
   <si>
-    <t>Bulgaria closed its borders to non-EU/EEA nationals on March 20. In addition, travellers from France, Germany, Italy, the Netherlands, Spain, Switzerland, and the United Kingdom cannot enter the country.  Bulgarian citizens and permanent residents and their families are exempt. Turkey closed its border to Greek and Bulgarian citizens on March 18.</t>
-  </si>
-  <si>
-    <t>Nurseries, kindergartens, schools and universities closed. These measures are to remain in place until April 13.</t>
+    <t>Bulgaria closed its borders to non-EU/EEA nationals on March 20. In addition, travellers from France, Germany, Italy, the Netherlands, Spain, Switzerland, and the United Kingdom cannot enter the country.  Bulgarian citizens and permanent residents and their families are exempt. Turkey closed its border to Greek and Bulgarian citizens on 18 March.</t>
+  </si>
+  <si>
+    <t>Nurseries, kindergartens, schools and universities closed. These measures are to remain in place until 13 April.</t>
   </si>
   <si>
     <t xml:space="preserve">Shops in shopping centres, restaurants, amusement/gambling halls, bars and nightclubs shut. Banks, insurance offices, grocery stores and pharmacies remain open. Mass events stopped and sports, cultural and entertainment premises (cinemas, theatres, concerts, museums, conferences, symposia, sports centres, gyms, etc.) are to be closed. All employers, if possible, are to introduce remote work for their employees. </t>
   </si>
   <si>
-    <t>Routine medical consultations, examinations, immunizations, planned operations, and visits to all medical establishments have been stopped. Visits to nursing homes no longer allowed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The government's priority has been to increase funding for the health sector response. The total amount of government support to the private sector and households is estimated to be around BGN 4.6 billion. The government is yet to announce the details of the major private sector support programs for employment and firm liquidity. The government indicated that the 2020 budget is likely to be updated. </t>
+    <t>Routine medical consultations, examinations, immunizations, planned operations, and visits to all medical establishments have been stopped. Visits to nursing homes not allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The government's priority has been to increase funding for the health sector response. The total amount of government support to the private sector and households is estimated to be around BGN 4.6 billion (Eur 2.35 billion). The government is yet to announce the details of the major private sector support programs for employment and firm liquidity. The government indicated that the 2020 budget is likely to be updated. </t>
   </si>
   <si>
     <t xml:space="preserve">Employees can be requested to use half of their annual paid leave during the State of Emergency. In addition, the government will pay 60% of salaries for employees for three months facing being laid off, with employers paying the remaining 40%. The details on which companies can access this state assistance are to be drafted by the Cabinet. Expenditure on support for job retention in the sectors concerned is to reach BGN 1 billion (EUR 510 million). Doctors and nurses working in the frontline will receive an additional payment of BGN 1000 a month (EUR 510). The additional remuneration of medical and non-medical staff involved in the treatment of COVID 19 patients is estimated to BGN 60 million (EUR 30.6 million). The government will allocate BGN 200 million (EUR 102 million) to the Bulgarian Development Bank (BDB) for guaranteeing non-interest consumer loans up to BGN 1500 (EUR 765) for employees who have gone on unpaid leave. Certain taxes and fees due to the government have been delayed. This includes the deadline for submission of the annual income tax return and for payment of the tax assessed, which have been extended until end-June for firms/sole traders involved in commerce and for farmers who pay taxes under this regime. </t>
@@ -603,7 +604,7 @@
 Self-employed will be given a six-month waiver on the (minimum) payments of health and social insurance (May to August). 
 The government has also approved a targeted employment support programme (Antivirus), to compensate for all or part of salary costs for the time of the quarantine or emergency measures (from 1st March). Employees ordered into quarantine will receive 60 % of their salaries and the government will reimburse the company in full. Employers, who had to close or reduce operations because of the crisis measures, will pay employees their full salaries, and the state will reimburse employers 80 % of the costs. Employees in firms facing inputs supply issues or drop in sales will receive 80%, resp. 60%, of their salaries with the state reimbursing 50% of the cost in both cases. The Ministry of Labour and Social Affairs expects the total costs of the Program to be 1.2bn. CZK (0.02 % of GDP).
 Other proposed measures include: Waiver of the advance payments (not the tax itself) for corporate and personal income tax in June. Introduction of the institute of tax return retroactivity - entrepreneurs will be able to recover any loss reported in 2020 in their tax bases in 2019 and 2018, thereby obtaining a refund from the Financial Administration.
-The Government released 3.3 billion CZK for the 2020 Rural Development Program. This funding should help entrepreneurs in agriculture, food and forestry while fighting coronavirus crisis. The main reason for this support is ensuring the Czech food independency. The government has introduced waivers of any penalties and default interest for corporate and personal income tax payments up to 1 July.
+The Government released CZK 3.3 billion for the 2020 Rural Development Program. This funding should help entrepreneurs in agriculture, food and forestry while fighting coronavirus crisis. The main reason for this support is ensuring the Czech food independency. The Government has also increased funds by CZK 1 bn for the Support and Guarantee Farm and Forestry Fund, to provide farmers and foresters with more liquidity (delay of loan repayments).                                                                                   The government has introduced waivers of any penalties and default interest for corporate and personal income tax payments up to 1 July.
 </t>
   </si>
   <si>
@@ -756,7 +757,7 @@
 • Supplemental credit of EUR 25 million to cover meal allowances to ensure the basic access to food for vulnerable children affected by the suspension of educational activity in schools.
 • Additional flexibility for local authorities to use their 2019 budgetary surplus to fund social services and primary assistance to dependent persons (EUR 300 million) 
 • The social benefit for energy provision (‘bono social’) will be automatically extended until September 15.
-• Dismissals for reasons realted to Covid19 will not be considered justified (from March 27 till the end of the health crisis)
+• Dismissals for reasons related to Covid19 will not be considered justified (from March 27 until the end of the health crisis)
 Other employment and social measures:
 • One-month credit postponement on mortgage payments for the most vulnerable.
 • Broadened scope for protected families in the supply of water and energy, which is ensured for vulnerable groups. Telecommunication services are also guaranteed.
@@ -1097,18 +1098,19 @@
   </si>
   <si>
     <t>- The government plans to reduce the number of restricted import goods by up to 50 percent on steel producers, and their derivatives, strategic food products (manufacturing industry inputs); horticultural commodities; animals &amp; animal products; medicine, medicinal ingredients &amp; food.
-- Presidential Instruction Number 4/2020 issued on 23 March 2020 on Refocusing of Activities, Budget Reallocation, and Public Procurement in response to handle the Covid-19 in Indonesia.</t>
-  </si>
-  <si>
-    <t>- Key dispositions of the second fiscal package include exempting some manufacturing workers from income tax 
-- Incentives for medical staff (IDR 15 million to medical specialists, IDR 10 million to physicians and dentists, IDR 7.5 million to nurses and IDR 5 million to other medical staff members)
-- Provide housing interest subsidies for the bottom 40% 
-- Adding possible beneficieries and increase the number of basic food cards from 150,000 IDR to 200,000 IDR for six months</t>
+- Presidential Instruction Number 4/2020 issued on 23 March 2020 on Refocusing of Activities, Budget Reallocation, and Public Procurement in response to handle the Covid-19 in Indonesia. It results in reallocation representing IDR 62 trillion for state budget and IDR 72 trillion for village funds</t>
+  </si>
+  <si>
+    <t>- Key dispositions of the second fiscal package include exempting from income tax for six months manufacturing workers with annual income below IDR 200 million (budget of IDR 8.6 trillion) 
+- Incentives for medical staff dealing with covid-19 (IDR 15 million to medical specialists, IDR 10 million to physicians and dentists, IDR 7.5 million to nurses and IDR 5 million to other medical staff members; IDR 300 million in case of death of a medical worker) for a budget of IDR 6.1 trillion
+- Provide housing interest subsidies for the bottom 40% (budget of IDR 1.5 trillion)
+- Adding possible beneficieries and increase the number of basic food cards from 150,000 IDR to 200,000 IDR for six months (budget of IDR 4.6 trillion)</t>
   </si>
   <si>
     <t>- The first fiscal stimulus provide flight ticket incentive to 10 tourism destinations as well as taxincentive to hotels and restaurants
-- The second fiscal package includes reducing corporate tax payments for manufacturing companies.
-- Incentives for MSMEs</t>
+- The second fiscal package includes reducing corporate tax payments for manufacturing companies (IDR 12.5 trillion).
+- Incentives for MSMEs
+- Easier repayment for overpaid taxes (IDR 2 trillion)</t>
   </si>
   <si>
     <t>- BI announced on March 9 five measures to stabilize the rupiah – including cutting the USD reserve requirement ratio (RRR) to 4% from 8% and the rupiah RRR by 50 basis points, starting April 1 (only for banks with clients engaged in export and import activities). 
@@ -1686,8 +1688,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">- 585 cases, 8 deaths.
-- At 5.8% of GDP, Mexico allocates a relatively low share of its national resources to health, compared with the OECD average of 9% though it is similar to countries with comparable GDP levels. Spending remains concentrated in the richest states, resulting in disparities in care quality and access. The system suffers from fragmentation. 
+    <t xml:space="preserve">- At 5.8% of GDP, Mexico allocates a relatively low share of its national resources to health, compared with the OECD average of 9% though it is similar to countries with comparable GDP levels. Spending remains concentrated in the richest states, resulting in disparities in care quality and access. The system suffers from fragmentation. 
 - The President announced on 12 March that military medical workers and facilities would be part of the response to the pandemic.
 - On 24 March, the President announced additional resources for the Secretary of National Defence (SEDENA) and the Secretary of the Navy (SEMAR) of 4 000 million MXN (164.5 million USD) and 500 million MXN (20.5 million USD), respectively. 
 - States will receive in transfers from the Federal Government of 15 300 million MXN (629 million USD) through the Health and Well-being Institute. Furthermore, states will receive advance funding for 10 000 million MXN (411 million USD).  
@@ -1895,7 +1896,7 @@
   </si>
   <si>
     <t>In the context of the Covid-19 support measures announced on 17 March, NZD 500 million was allocated to the health sector.   
-On 28 arch the government amounced that it will temporarily remove tariffs on all medical and hygiene imports needed for the COVID-19 response. These include all diagnostic reagents and testing kits used for COVID-19 testing and soap imports.</t>
+On 28 March, the government announced that it will temporarily remove tariffs on all medical and hygiene imports needed for the COVID-19 response. These include all diagnostic reagents and testing kits used for COVID-19 testing and soap imports.</t>
   </si>
   <si>
     <t xml:space="preserve">The government announced a massive package of support measures on 17 March amounting to NZD 12.1 billion (4% of GDP), with one half to be implemented in the coming year. Most (NZD 8.7 billion) of the fiscal measures are to support businesses and jobs while NZD 2.8 billion were allocated to increase social benefit payments and NZD 500 million (0.2% of GDP) were allocated to the health sector. The package is expected to boost GDP growth by 2 percentage points in the coming year and by further small amounts over the following two years. This package comes on top of the NZD 12 billion increase in infrastructure spending announced in January.     </t>
@@ -2167,16 +2168,36 @@
     <t>All educational institutions are closed</t>
   </si>
   <si>
-    <t>All public indoor events with more than 500 visitors have been banned. On 18/3-2020 all public gatherings were limited to 5 people.</t>
-  </si>
-  <si>
-    <t>An army filed hospital has been deployed in Ljubljana. In addition, health professionals are prohibited from travelling abroad and their right to leave and strike is restricted</t>
-  </si>
-  <si>
-    <t>- EUR 1 billion stimulus package to mitigate the impact on the economy</t>
-  </si>
-  <si>
-    <t>- Stimulus package includes short- and long-term measures such as tax deferrals, state guarantees and credit lines. On 18/3-2020, the tax burden on business was eased with a 12 month deferral of credit payments.</t>
+    <t>All public indoor events with more than 500 visitors have been banned. On 18/3-2020 all public gatherings were limited to 5 people.
+All, except grocery, shops, bars and restaurants, hotels, and services establishments have been shut down. Petrol stations and pharmacies remain open.
+Grocery shops must be open from 8am to 8pm. Until 10 am, priority must be given to vulnerable groups, including the elderly, pregnant women and disabled persons.</t>
+  </si>
+  <si>
+    <t>An army filed hospital has been deployed in Ljubljana. In addition, health professionals are prohibited from travelling abroad and their right to leave and strike is restricted.
+The government has set maximum prices for protective medical gear and other medical equipment</t>
+  </si>
+  <si>
+    <t>EUR 1 billion stimulus package to mitigate the impact on the economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The government will until the end of May pay compensation for temporary lay-offs and trade restrictions for agriculture and food products, including for the self-employed, and reimburse employees in companies that are forced to fully or partially suspend their operations their lost salaries. 
+The government will pay all social security contributions for firms that continue operations during the crisis, and co-finance 20% of employees’ net compensation. 
+For Covid-19 patients, the national health insurance fund will finance employers’ obligation to pay sick leave for the first 30 days of sickness for people falling sick during the crisis.
+Measures for public employees include performance based salary increases (up to 200%) in areas that are key to overcome the epidemic (such as health care, security, etc.).  Salaries of state officials at the national level and of members of SOE boards are reduced by 30% for the duration of epidemic.
+Unemployed are entitled to benefits from the first day of unemployment. Self-employed have been guaranteed a minimum income of 70% of the net minimum wage and no longer subject to social security contributions.
+The government provides 40% co-financing of wage compensation for temporary layoffs and for employees that cease to work because of force majeure factors to secure 80% compensation. The measure will be valid for two months.  In case of quarantine, the state covers 80% of wages.
+Parents who stay home to care for their children are entitled to a 50% wage compensation. 
+A crisis bonus is available to pensioners and the most vulnerable groups of the population.
+</t>
+  </si>
+  <si>
+    <t>Stimulus package includes short- and long-term measures such as tax deferrals, state guarantees and credit lines.
+The tax burden on business was eased with a 12 month deferral of credit payments.
+Corporate income tax payments has be deferred for up to 24 months without incurring interest. 
+Credit payments to the state has been deferred by 12 months. 
+State suppliers will be paid within 8 days instead of a minimum of 30 days. 
+Income tax payment is deferred until the 2020 income tax assessment.
+The state-owned export and development bank will make additional funding, totaling 2¾ % of GDP, available</t>
   </si>
   <si>
     <t>SWE</t>
@@ -3553,7 +3574,7 @@
       </c>
       <c r="L6" s="22"/>
     </row>
-    <row r="7" spans="1:12" s="17" customFormat="1" ht="318.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>33</v>
       </c>
@@ -5061,7 +5082,7 @@
       </c>
       <c r="L49" s="22"/>
     </row>
-    <row r="50" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
         <v>445</v>
       </c>
@@ -5084,207 +5105,209 @@
       <c r="H50" s="23" t="s">
         <v>450</v>
       </c>
-      <c r="I50" s="23"/>
+      <c r="I50" s="23" t="s">
+        <v>451</v>
+      </c>
       <c r="J50" s="23" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K50" s="23"/>
       <c r="L50" s="22"/>
     </row>
     <row r="51" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B51" s="18">
         <v>43920</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="L51" s="22"/>
     </row>
     <row r="52" spans="1:12" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B52" s="18">
         <v>43920</v>
       </c>
       <c r="C52" s="22"/>
       <c r="D52" s="23" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="23" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I52" s="23"/>
       <c r="J52" s="23"/>
       <c r="K52" s="23" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="L52" s="22"/>
     </row>
     <row r="53" spans="1:12" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B53" s="18">
         <v>43920</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I53" s="17" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="K53" s="17" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="L53" s="22"/>
     </row>
     <row r="54" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B54" s="18">
         <v>43920</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="L54" s="22"/>
     </row>
     <row r="55" spans="1:12" s="17" customFormat="1" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B55" s="18">
         <v>43920</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="17" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="19"/>
       <c r="H55" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="J55" s="21"/>
       <c r="K55" s="17" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="L55" s="22"/>
     </row>
     <row r="56" spans="1:12" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B56" s="18">
         <v>43920</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="J56" s="23" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="L56" s="22"/>
     </row>

</xml_diff>